<commit_message>
Agregado parte de hash
</commit_message>
<xml_diff>
--- a/tiempos-VNS.xlsx
+++ b/tiempos-VNS.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="439">
   <si>
     <t>Nombre de la instancia</t>
   </si>
@@ -26,46 +26,55 @@
     <t>GKD-a_10_n10_m3.txt</t>
   </si>
   <si>
-    <t>428.56418</t>
-  </si>
-  <si>
-    <t>-1.51446909E15</t>
+    <t>425.74805</t>
+  </si>
+  <si>
+    <t>-8.0024611E18</t>
   </si>
   <si>
     <t>GKD-a_11_n10_m4.txt</t>
   </si>
   <si>
-    <t>679.2232</t>
-  </si>
-  <si>
-    <t>-1.51446922E15</t>
+    <t>614.5233</t>
+  </si>
+  <si>
+    <t>-8.0318967E18</t>
   </si>
   <si>
     <t>GKD-a_12_n10_m4.txt</t>
   </si>
   <si>
-    <t>1131.6687</t>
+    <t>1133.1014</t>
+  </si>
+  <si>
+    <t>-8.0460925E18</t>
   </si>
   <si>
     <t>GKD-a_13_n10_m4.txt</t>
   </si>
   <si>
-    <t>761.8519</t>
-  </si>
-  <si>
-    <t>-1.51446936E15</t>
+    <t>713.41534</t>
+  </si>
+  <si>
+    <t>-8.0592921E18</t>
   </si>
   <si>
     <t>GKD-a_14_n10_m4.txt</t>
   </si>
   <si>
-    <t>1043.0114</t>
+    <t>999.4699</t>
+  </si>
+  <si>
+    <t>-8.5254026E18</t>
   </si>
   <si>
     <t>GKD-a_15_n10_m4.txt</t>
   </si>
   <si>
-    <t>1195.7017</t>
+    <t>1193.3375</t>
+  </si>
+  <si>
+    <t>-8.5397001E18</t>
   </si>
   <si>
     <t>GKD-a_16_n10_m6.txt</t>
@@ -74,28 +83,34 @@
     <t>2106.7388</t>
   </si>
   <si>
-    <t>-1.51446949E15</t>
+    <t>-8.5550718E18</t>
   </si>
   <si>
     <t>GKD-a_17_n10_m6.txt</t>
   </si>
   <si>
-    <t>2327.4023</t>
+    <t>2348.6746</t>
+  </si>
+  <si>
+    <t>-8.5727525E18</t>
   </si>
   <si>
     <t>GKD-a_18_n10_m6.txt</t>
   </si>
   <si>
-    <t>1826.9965</t>
-  </si>
-  <si>
-    <t>-1.51446962E15</t>
+    <t>1722.483</t>
+  </si>
+  <si>
+    <t>-8.5856289E18</t>
   </si>
   <si>
     <t>GKD-a_19_n10_m6.txt</t>
   </si>
   <si>
-    <t>2446.5215</t>
+    <t>2452.1162</t>
+  </si>
+  <si>
+    <t>-8.5986966E18</t>
   </si>
   <si>
     <t>GKD-a_1_n10_m2.txt</t>
@@ -104,67 +119,79 @@
     <t>199.05042</t>
   </si>
   <si>
+    <t>-8.6114564E18</t>
+  </si>
+  <si>
     <t>GKD-a_20_n10_m6.txt</t>
   </si>
   <si>
-    <t>1386.2245</t>
-  </si>
-  <si>
-    <t>-1.51446976E15</t>
+    <t>1366.2219</t>
+  </si>
+  <si>
+    <t>-8.6212058E18</t>
   </si>
   <si>
     <t>GKD-a_21_n10_m8.txt</t>
   </si>
   <si>
-    <t>5275.5737</t>
+    <t>5231.4253</t>
+  </si>
+  <si>
+    <t>-8.6324049E18</t>
   </si>
   <si>
     <t>GKD-a_22_n10_m8.txt</t>
   </si>
   <si>
-    <t>3387.8435</t>
-  </si>
-  <si>
-    <t>-1.51446989E15</t>
+    <t>3387.8433</t>
+  </si>
+  <si>
+    <t>-8.6464506E18</t>
   </si>
   <si>
     <t>GKD-a_23_n10_m8.txt</t>
   </si>
   <si>
-    <t>2720.6113</t>
+    <t>2665.6746</t>
+  </si>
+  <si>
+    <t>-8.6832128E18</t>
   </si>
   <si>
     <t>GKD-a_24_n10_m8.txt</t>
   </si>
   <si>
-    <t>3506.0864</t>
-  </si>
-  <si>
-    <t>-1.51447003E15</t>
+    <t>3506.087</t>
+  </si>
+  <si>
+    <t>-8.6982695E18</t>
   </si>
   <si>
     <t>GKD-a_25_n10_m8.txt</t>
   </si>
   <si>
-    <t>3653.0437</t>
+    <t>3607.8909</t>
+  </si>
+  <si>
+    <t>-8.712628E18</t>
   </si>
   <si>
     <t>GKD-a_26_n15_m3.txt</t>
   </si>
   <si>
-    <t>335.10492</t>
-  </si>
-  <si>
-    <t>-1.51447016E15</t>
+    <t>299.89288</t>
+  </si>
+  <si>
+    <t>-8.7284588E18</t>
   </si>
   <si>
     <t>GKD-a_27_n15_m3.txt</t>
   </si>
   <si>
-    <t>653.53357</t>
-  </si>
-  <si>
-    <t>-1.5144703E15</t>
+    <t>648.6155</t>
+  </si>
+  <si>
+    <t>-8.7394385E18</t>
   </si>
   <si>
     <t>GKD-a_28_n15_m3.txt</t>
@@ -173,13 +200,16 @@
     <t>625.14844</t>
   </si>
   <si>
+    <t>-8.749902E18</t>
+  </si>
+  <si>
     <t>GKD-a_29_n15_m3.txt</t>
   </si>
   <si>
-    <t>497.8221</t>
-  </si>
-  <si>
-    <t>-1.51447043E15</t>
+    <t>487.6406</t>
+  </si>
+  <si>
+    <t>-8.7645101E18</t>
   </si>
   <si>
     <t>GKD-a_2_n10_m2.txt</t>
@@ -188,19 +218,25 @@
     <t>171.92285</t>
   </si>
   <si>
+    <t>-8.7772133E18</t>
+  </si>
+  <si>
     <t>GKD-a_30_n15_m3.txt</t>
   </si>
   <si>
-    <t>575.1362</t>
-  </si>
-  <si>
-    <t>-1.51447056E15</t>
+    <t>575.13617</t>
+  </si>
+  <si>
+    <t>-8.7871457E18</t>
   </si>
   <si>
     <t>GKD-a_31_n15_m4.txt</t>
   </si>
   <si>
-    <t>584.4085</t>
+    <t>529.5569</t>
+  </si>
+  <si>
+    <t>-8.7984971E18</t>
   </si>
   <si>
     <t>GKD-a_32_n15_m4.txt</t>
@@ -209,118 +245,142 @@
     <t>875.77325</t>
   </si>
   <si>
-    <t>-1.5144707E15</t>
+    <t>-8.808131E18</t>
   </si>
   <si>
     <t>GKD-a_33_n15_m4.txt</t>
   </si>
   <si>
-    <t>1243.5947</t>
+    <t>1177.2147</t>
+  </si>
+  <si>
+    <t>-8.8180316E18</t>
   </si>
   <si>
     <t>GKD-a_34_n15_m4.txt</t>
   </si>
   <si>
-    <t>824.35236</t>
-  </si>
-  <si>
-    <t>-1.51447083E15</t>
+    <t>805.3876</t>
+  </si>
+  <si>
+    <t>-8.8277782E18</t>
   </si>
   <si>
     <t>GKD-a_35_n15_m4.txt</t>
   </si>
   <si>
-    <t>529.7877</t>
-  </si>
-  <si>
-    <t>-1.51447097E15</t>
+    <t>472.22815</t>
+  </si>
+  <si>
+    <t>-8.8481439E18</t>
   </si>
   <si>
     <t>GKD-a_36_n15_m6.txt</t>
   </si>
   <si>
-    <t>2801.8933</t>
-  </si>
-  <si>
-    <t>-1.5144711E15</t>
+    <t>2743.1511</t>
+  </si>
+  <si>
+    <t>-8.8611121E18</t>
   </si>
   <si>
     <t>GKD-a_37_n15_m6.txt</t>
   </si>
   <si>
-    <t>2829.6033</t>
+    <t>2758.3184</t>
+  </si>
+  <si>
+    <t>-8.8842172E18</t>
   </si>
   <si>
     <t>GKD-a_38_n15_m6.txt</t>
   </si>
   <si>
-    <t>2223.6106</t>
+    <t>2059.7966</t>
+  </si>
+  <si>
+    <t>-8.8942233E18</t>
   </si>
   <si>
     <t>GKD-a_39_n15_m6.txt</t>
   </si>
   <si>
-    <t>3082.8552</t>
-  </si>
-  <si>
-    <t>-1.51447124E15</t>
+    <t>2917.2737</t>
+  </si>
+  <si>
+    <t>-8.9053993E18</t>
   </si>
   <si>
     <t>GKD-a_3_n10_m2.txt</t>
   </si>
   <si>
-    <t>122.00874</t>
+    <t>146.61536</t>
+  </si>
+  <si>
+    <t>-8.919599E18</t>
   </si>
   <si>
     <t>GKD-a_40_n15_m6.txt</t>
   </si>
   <si>
-    <t>2416.7737</t>
-  </si>
-  <si>
-    <t>-1.51447137E15</t>
+    <t>2339.4866</t>
+  </si>
+  <si>
+    <t>-8.9268189E18</t>
   </si>
   <si>
     <t>GKD-a_41_n15_m9.txt</t>
   </si>
   <si>
-    <t>7250.224</t>
+    <t>7230.3447</t>
+  </si>
+  <si>
+    <t>-8.9377893E18</t>
   </si>
   <si>
     <t>GKD-a_42_n15_m9.txt</t>
   </si>
   <si>
-    <t>6366.322</t>
+    <t>6298.024</t>
+  </si>
+  <si>
+    <t>-8.9502204E18</t>
   </si>
   <si>
     <t>GKD-a_43_n15_m9.txt</t>
   </si>
   <si>
-    <t>4226.928</t>
-  </si>
-  <si>
-    <t>-1.5144715E15</t>
+    <t>4095.7732</t>
+  </si>
+  <si>
+    <t>-8.9612891E18</t>
   </si>
   <si>
     <t>GKD-a_44_n15_m9.txt</t>
   </si>
   <si>
-    <t>5697.1514</t>
+    <t>5436.9375</t>
+  </si>
+  <si>
+    <t>-8.972215E18</t>
   </si>
   <si>
     <t>GKD-a_45_n15_m9.txt</t>
   </si>
   <si>
-    <t>4157.681</t>
-  </si>
-  <si>
-    <t>-1.51447164E15</t>
+    <t>4115.4004</t>
+  </si>
+  <si>
+    <t>-8.9880056E18</t>
   </si>
   <si>
     <t>GKD-a_46_n15_m12.txt</t>
   </si>
   <si>
-    <t>10317.745</t>
+    <t>10305.452</t>
+  </si>
+  <si>
+    <t>-9.0001283E18</t>
   </si>
   <si>
     <t>GKD-a_47_n15_m12.txt</t>
@@ -329,211 +389,268 @@
     <t>13080.442</t>
   </si>
   <si>
+    <t>-9.0159178E18</t>
+  </si>
+  <si>
     <t>GKD-a_48_n15_m12.txt</t>
   </si>
   <si>
-    <t>11080.221</t>
-  </si>
-  <si>
-    <t>-1.51447177E15</t>
+    <t>11051.198</t>
+  </si>
+  <si>
+    <t>-9.030654E18</t>
   </si>
   <si>
     <t>GKD-a_49_n15_m12.txt</t>
   </si>
   <si>
-    <t>7872.438</t>
+    <t>7833.0103</t>
+  </si>
+  <si>
+    <t>-9.0496558E18</t>
   </si>
   <si>
     <t>GKD-a_4_n10_m2.txt</t>
   </si>
   <si>
-    <t>186.18103</t>
-  </si>
-  <si>
-    <t>-1.51447191E15</t>
+    <t>171.31491</t>
+  </si>
+  <si>
+    <t>-9.0843696E18</t>
   </si>
   <si>
     <t>GKD-a_50_n15_m12.txt</t>
   </si>
   <si>
-    <t>10274.558</t>
+    <t>10040.516</t>
+  </si>
+  <si>
+    <t>-9.0970766E18</t>
   </si>
   <si>
     <t>GKD-a_51_n30_m6.txt</t>
   </si>
   <si>
-    <t>3138.0325</t>
-  </si>
-  <si>
-    <t>-1.51447204E15</t>
+    <t>2989.2014</t>
+  </si>
+  <si>
+    <t>-9.1123895E18</t>
   </si>
   <si>
     <t>GKD-a_52_n30_m6.txt</t>
   </si>
   <si>
-    <t>3262.646</t>
+    <t>2975.556</t>
+  </si>
+  <si>
+    <t>-9.1216733E18</t>
   </si>
   <si>
     <t>GKD-a_53_n30_m6.txt</t>
   </si>
   <si>
-    <t>2614.2366</t>
+    <t>2591.3767</t>
+  </si>
+  <si>
+    <t>-9.1310219E18</t>
   </si>
   <si>
     <t>GKD-a_54_n30_m6.txt</t>
   </si>
   <si>
-    <t>1894.9673</t>
-  </si>
-  <si>
-    <t>-1.51447217E15</t>
+    <t>1839.6672</t>
+  </si>
+  <si>
+    <t>-9.1418158E18</t>
   </si>
   <si>
     <t>GKD-a_55_n30_m6.txt</t>
   </si>
   <si>
-    <t>1859.7645</t>
+    <t>1747.2439</t>
+  </si>
+  <si>
+    <t>-9.1508884E18</t>
   </si>
   <si>
     <t>GKD-a_56_n30_m9.txt</t>
   </si>
   <si>
-    <t>5873.8706</t>
+    <t>5912.867</t>
+  </si>
+  <si>
+    <t>-9.1604684E18</t>
   </si>
   <si>
     <t>GKD-a_57_n30_m9.txt</t>
   </si>
   <si>
-    <t>7664.2007</t>
-  </si>
-  <si>
-    <t>-1.51447231E15</t>
+    <t>7573.15</t>
+  </si>
+  <si>
+    <t>-9.1714003E18</t>
   </si>
   <si>
     <t>GKD-a_58_n30_m9.txt</t>
   </si>
   <si>
-    <t>6365.286</t>
+    <t>6250.9365</t>
+  </si>
+  <si>
+    <t>-9.181479E18</t>
   </si>
   <si>
     <t>GKD-a_59_n30_m9.txt</t>
   </si>
   <si>
-    <t>7178.511</t>
+    <t>7141.182</t>
+  </si>
+  <si>
+    <t>-9.1931696E18</t>
   </si>
   <si>
     <t>GKD-a_5_n10_m2.txt</t>
   </si>
   <si>
-    <t>207.357</t>
-  </si>
-  <si>
-    <t>-1.51447244E15</t>
+    <t>199.19339</t>
+  </si>
+  <si>
+    <t>-9.2049332E18</t>
   </si>
   <si>
     <t>GKD-a_60_n30_m9.txt</t>
   </si>
   <si>
-    <t>6732.254</t>
+    <t>6780.777</t>
+  </si>
+  <si>
+    <t>-9.2113907E18</t>
   </si>
   <si>
     <t>GKD-a_61_n30_m12.txt</t>
   </si>
   <si>
-    <t>12710.449</t>
+    <t>12692.514</t>
+  </si>
+  <si>
+    <t>-9.2213682E18</t>
   </si>
   <si>
     <t>GKD-a_62_n30_m12.txt</t>
   </si>
   <si>
-    <t>9723.184</t>
-  </si>
-  <si>
-    <t>-1.51447258E15</t>
+    <t>9321.555</t>
+  </si>
+  <si>
+    <t>9.214543E18</t>
   </si>
   <si>
     <t>GKD-a_63_n30_m12.txt</t>
   </si>
   <si>
-    <t>13220.446</t>
+    <t>13047.45</t>
+  </si>
+  <si>
+    <t>9.2023439E18</t>
   </si>
   <si>
     <t>GKD-a_64_n30_m12.txt</t>
   </si>
   <si>
-    <t>10961.321</t>
-  </si>
-  <si>
-    <t>-1.51447271E15</t>
+    <t>10957.046</t>
+  </si>
+  <si>
+    <t>9.1878523E18</t>
   </si>
   <si>
     <t>GKD-a_65_n30_m12.txt</t>
   </si>
   <si>
-    <t>9012.124</t>
+    <t>8669.129</t>
+  </si>
+  <si>
+    <t>9.1742019E18</t>
   </si>
   <si>
     <t>GKD-a_66_n30_m18.txt</t>
   </si>
   <si>
-    <t>24270.959</t>
+    <t>24274.27</t>
+  </si>
+  <si>
+    <t>9.1623074E18</t>
   </si>
   <si>
     <t>GKD-a_67_n30_m18.txt</t>
   </si>
   <si>
-    <t>23099.94</t>
-  </si>
-  <si>
-    <t>-1.51447285E15</t>
+    <t>23247.967</t>
+  </si>
+  <si>
+    <t>9.1477443E18</t>
   </si>
   <si>
     <t>GKD-a_68_n30_m18.txt</t>
   </si>
   <si>
-    <t>28963.697</t>
+    <t>29228.793</t>
+  </si>
+  <si>
+    <t>9.1329702E18</t>
   </si>
   <si>
     <t>GKD-a_69_n30_m18.txt</t>
   </si>
   <si>
-    <t>25595.975</t>
-  </si>
-  <si>
-    <t>-1.51447298E15</t>
+    <t>25250.441</t>
+  </si>
+  <si>
+    <t>9.1185924E18</t>
   </si>
   <si>
     <t>GKD-a_6_n10_m3.txt</t>
   </si>
   <si>
-    <t>216.42151</t>
+    <t>245.22943</t>
+  </si>
+  <si>
+    <t>9.1015038E18</t>
   </si>
   <si>
     <t>GKD-a_70_n30_m18.txt</t>
   </si>
   <si>
-    <t>23088.104</t>
+    <t>22766.244</t>
+  </si>
+  <si>
+    <t>9.0920216E18</t>
   </si>
   <si>
     <t>GKD-a_71_n30_m24.txt</t>
   </si>
   <si>
-    <t>33708.027</t>
-  </si>
-  <si>
-    <t>-1.51447311E15</t>
+    <t>33762.156</t>
+  </si>
+  <si>
+    <t>9.072784E18</t>
   </si>
   <si>
     <t>GKD-a_72_n30_m24.txt</t>
   </si>
   <si>
-    <t>49708.223</t>
+    <t>49298.74</t>
+  </si>
+  <si>
+    <t>9.0533408E18</t>
   </si>
   <si>
     <t>GKD-a_73_n30_m24.txt</t>
   </si>
   <si>
-    <t>26855.5</t>
+    <t>27166.15</t>
+  </si>
+  <si>
+    <t>9.034101E18</t>
   </si>
   <si>
     <t>GKD-a_74_n30_m24.txt</t>
@@ -542,55 +659,70 @@
     <t>18941.016</t>
   </si>
   <si>
-    <t>-1.51447325E15</t>
+    <t>9.0155374E18</t>
   </si>
   <si>
     <t>GKD-a_75_n30_m24.txt</t>
   </si>
   <si>
-    <t>16420.41</t>
+    <t>16420.406</t>
+  </si>
+  <si>
+    <t>8.9969738E18</t>
   </si>
   <si>
     <t>GKD-a_7_n10_m3.txt</t>
   </si>
   <si>
-    <t>468.35406</t>
-  </si>
-  <si>
-    <t>-1.51447338E15</t>
+    <t>468.68372</t>
+  </si>
+  <si>
+    <t>8.9794927E18</t>
   </si>
   <si>
     <t>GKD-a_8_n10_m3.txt</t>
   </si>
   <si>
-    <t>354.06345</t>
+    <t>339.89642</t>
+  </si>
+  <si>
+    <t>8.9733975E18</t>
   </si>
   <si>
     <t>GKD-a_9_n10_m3.txt</t>
   </si>
   <si>
-    <t>551.3875</t>
+    <t>541.0896</t>
+  </si>
+  <si>
+    <t>8.9668307E18</t>
   </si>
   <si>
     <t>GKD-b_10_n25_m7.txt</t>
   </si>
   <si>
-    <t>3298.0889</t>
-  </si>
-  <si>
-    <t>-1.51447352E15</t>
+    <t>3343.05</t>
+  </si>
+  <si>
+    <t>8.9585167E18</t>
   </si>
   <si>
     <t>GKD-b_11_n50_m5.txt</t>
   </si>
   <si>
-    <t>1721.893</t>
+    <t>1687.4786</t>
+  </si>
+  <si>
+    <t>8.9480582E18</t>
   </si>
   <si>
     <t>GKD-b_12_n50_m5.txt</t>
   </si>
   <si>
-    <t>1985.3248</t>
+    <t>2041.5875</t>
+  </si>
+  <si>
+    <t>8.9388305E18</t>
   </si>
   <si>
     <t>GKD-b_13_n50_m5.txt</t>
@@ -599,289 +731,358 @@
     <t>1296.7046</t>
   </si>
   <si>
+    <t>8.9220344E18</t>
+  </si>
+  <si>
     <t>GKD-b_14_n50_m5.txt</t>
   </si>
   <si>
-    <t>1251.2135</t>
-  </si>
-  <si>
-    <t>-1.51447365E15</t>
+    <t>1162.5571</t>
+  </si>
+  <si>
+    <t>8.9137479E18</t>
   </si>
   <si>
     <t>GKD-b_15_n50_m5.txt</t>
   </si>
   <si>
-    <t>1854.4268</t>
+    <t>1834.3105</t>
+  </si>
+  <si>
+    <t>8.9062404E18</t>
   </si>
   <si>
     <t>GKD-b_16_n50_m15.txt</t>
   </si>
   <si>
-    <t>10258.991</t>
+    <t>10559.1045</t>
+  </si>
+  <si>
+    <t>8.8978226E18</t>
   </si>
   <si>
     <t>GKD-b_17_n50_m15.txt</t>
   </si>
   <si>
-    <t>7521.0806</t>
-  </si>
-  <si>
-    <t>-1.51447379E15</t>
+    <t>7476.875</t>
+  </si>
+  <si>
+    <t>8.8855251E18</t>
   </si>
   <si>
     <t>GKD-b_18_n50_m15.txt</t>
   </si>
   <si>
-    <t>13198.489</t>
-  </si>
-  <si>
-    <t>-1.51447607E15</t>
+    <t>13283.816</t>
+  </si>
+  <si>
+    <t>8.8732644E18</t>
   </si>
   <si>
     <t>GKD-b_19_n50_m15.txt</t>
   </si>
   <si>
-    <t>14206.28</t>
+    <t>14129.346</t>
+  </si>
+  <si>
+    <t>8.8610247E18</t>
   </si>
   <si>
     <t>GKD-b_1_n25_m2.txt</t>
   </si>
   <si>
-    <t>109.9808</t>
+    <t>121.24863</t>
+  </si>
+  <si>
+    <t>8.8482791E18</t>
   </si>
   <si>
     <t>GKD-b_20_n50_m15.txt</t>
   </si>
   <si>
-    <t>13877.731</t>
-  </si>
-  <si>
-    <t>-1.5144762E15</t>
+    <t>13848.688</t>
+  </si>
+  <si>
+    <t>8.8430235E18</t>
   </si>
   <si>
     <t>GKD-b_21_n100_m10.txt</t>
   </si>
   <si>
-    <t>5066.8564</t>
+    <t>5011.751</t>
+  </si>
+  <si>
+    <t>8.8306749E18</t>
   </si>
   <si>
     <t>GKD-b_22_n100_m10.txt</t>
   </si>
   <si>
-    <t>7409.3867</t>
+    <t>7571.835</t>
+  </si>
+  <si>
+    <t>8.8198826E18</t>
   </si>
   <si>
     <t>GKD-b_23_n100_m10.txt</t>
   </si>
   <si>
-    <t>5289.9473</t>
+    <t>5010.535</t>
+  </si>
+  <si>
+    <t>8.8080442E18</t>
   </si>
   <si>
     <t>GKD-b_24_n100_m10.txt</t>
   </si>
   <si>
-    <t>9164.36</t>
-  </si>
-  <si>
-    <t>-1.51447634E15</t>
+    <t>8919.231</t>
+  </si>
+  <si>
+    <t>8.7964388E18</t>
   </si>
   <si>
     <t>GKD-b_25_n100_m10.txt</t>
   </si>
   <si>
-    <t>7371.7246</t>
+    <t>7303.9097</t>
+  </si>
+  <si>
+    <t>8.785679E18</t>
   </si>
   <si>
     <t>GKD-b_26_n100_m30.txt</t>
   </si>
   <si>
-    <t>46860.918</t>
-  </si>
-  <si>
-    <t>-1.51447647E15</t>
+    <t>46546.785</t>
+  </si>
+  <si>
+    <t>8.7740264E18</t>
   </si>
   <si>
     <t>GKD-b_27_n100_m30.txt</t>
   </si>
   <si>
-    <t>40178.523</t>
+    <t>40434.49</t>
+  </si>
+  <si>
+    <t>8.750189E18</t>
   </si>
   <si>
     <t>GKD-b_28_n100_m30.txt</t>
   </si>
   <si>
-    <t>91544.91</t>
+    <t>91750.914</t>
+  </si>
+  <si>
+    <t>8.7263351E18</t>
   </si>
   <si>
     <t>GKD-b_29_n100_m30.txt</t>
   </si>
   <si>
-    <t>80521.21</t>
-  </si>
-  <si>
-    <t>-1.5144766E15</t>
+    <t>79821.664</t>
+  </si>
+  <si>
+    <t>8.7016884E18</t>
   </si>
   <si>
     <t>GKD-b_2_n25_m2.txt</t>
   </si>
   <si>
-    <t>236.65034</t>
+    <t>247.39558</t>
+  </si>
+  <si>
+    <t>8.6777691E18</t>
   </si>
   <si>
     <t>GKD-b_30_n100_m30.txt</t>
   </si>
   <si>
-    <t>51575.473</t>
-  </si>
-  <si>
-    <t>-1.51447674E15</t>
+    <t>52626.938</t>
+  </si>
+  <si>
+    <t>8.6723705E18</t>
   </si>
   <si>
     <t>GKD-b_31_n125_m12.txt</t>
   </si>
   <si>
-    <t>4519.918</t>
+    <t>4684.7866</t>
+  </si>
+  <si>
+    <t>8.649295E18</t>
   </si>
   <si>
     <t>GKD-b_32_n125_m12.txt</t>
   </si>
   <si>
-    <t>12127.51</t>
+    <t>12272.461</t>
+  </si>
+  <si>
+    <t>8.6371515E18</t>
   </si>
   <si>
     <t>GKD-b_33_n125_m12.txt</t>
   </si>
   <si>
-    <t>7343.441</t>
-  </si>
-  <si>
-    <t>-1.51447687E15</t>
+    <t>7277.4355</t>
+  </si>
+  <si>
+    <t>8.6248688E18</t>
   </si>
   <si>
     <t>GKD-b_34_n125_m12.txt</t>
   </si>
   <si>
-    <t>12422.293</t>
+    <t>12518.147</t>
+  </si>
+  <si>
+    <t>8.6120161E18</t>
   </si>
   <si>
     <t>GKD-b_35_n125_m12.txt</t>
   </si>
   <si>
-    <t>6705.9727</t>
+    <t>6610.162</t>
+  </si>
+  <si>
+    <t>8.5977169E18</t>
   </si>
   <si>
     <t>GKD-b_36_n125_m37.txt</t>
   </si>
   <si>
-    <t>109646.87</t>
+    <t>109457.555</t>
+  </si>
+  <si>
+    <t>8.5848444E18</t>
   </si>
   <si>
     <t>GKD-b_37_n125_m37.txt</t>
   </si>
   <si>
-    <t>127043.72</t>
-  </si>
-  <si>
-    <t>-1.51447701E15</t>
+    <t>126930.59</t>
+  </si>
+  <si>
+    <t>8.5539036E18</t>
   </si>
   <si>
     <t>GKD-b_38_n125_m37.txt</t>
   </si>
   <si>
-    <t>87785.75</t>
-  </si>
-  <si>
-    <t>-1.51447714E15</t>
+    <t>88203.37</t>
+  </si>
+  <si>
+    <t>8.5233047E18</t>
   </si>
   <si>
     <t>GKD-b_39_n125_m37.txt</t>
   </si>
   <si>
-    <t>94656.15</t>
+    <t>94863.34</t>
+  </si>
+  <si>
+    <t>8.4924865E18</t>
   </si>
   <si>
     <t>GKD-b_3_n25_m2.txt</t>
   </si>
   <si>
-    <t>131.36134</t>
-  </si>
-  <si>
-    <t>-1.51447728E15</t>
+    <t>120.36586</t>
+  </si>
+  <si>
+    <t>8.4637937E18</t>
   </si>
   <si>
     <t>GKD-b_40_n125_m37.txt</t>
   </si>
   <si>
-    <t>119474.39</t>
+    <t>119214.914</t>
+  </si>
+  <si>
+    <t>8.4579393E18</t>
   </si>
   <si>
     <t>GKD-b_41_n150_m15.txt</t>
   </si>
   <si>
-    <t>21716.88</t>
-  </si>
-  <si>
-    <t>-1.51447741E15</t>
+    <t>21715.16</t>
+  </si>
+  <si>
+    <t>8.4114948E18</t>
   </si>
   <si>
     <t>GKD-b_42_n150_m15.txt</t>
   </si>
   <si>
-    <t>13310.768</t>
+    <t>13478.199</t>
+  </si>
+  <si>
+    <t>8.3824749E18</t>
   </si>
   <si>
     <t>GKD-b_43_n150_m15.txt</t>
   </si>
   <si>
-    <t>11728.886</t>
-  </si>
-  <si>
-    <t>-1.51447754E15</t>
+    <t>11674.483</t>
+  </si>
+  <si>
+    <t>8.3664066E18</t>
   </si>
   <si>
     <t>GKD-b_44_n150_m15.txt</t>
   </si>
   <si>
-    <t>15540.206</t>
+    <t>15432.11</t>
+  </si>
+  <si>
+    <t>8.3511212E18</t>
   </si>
   <si>
     <t>GKD-b_45_n150_m15.txt</t>
   </si>
   <si>
-    <t>15189.043</t>
+    <t>15556.826</t>
+  </si>
+  <si>
+    <t>8.3347462E18</t>
   </si>
   <si>
     <t>GKD-b_46_n150_m45.txt</t>
   </si>
   <si>
-    <t>155969.36</t>
-  </si>
-  <si>
-    <t>-1.51447768E15</t>
+    <t>156721.62</t>
+  </si>
+  <si>
+    <t>8.3154597E18</t>
   </si>
   <si>
     <t>GKD-b_47_n150_m45.txt</t>
   </si>
   <si>
-    <t>193493.78</t>
+    <t>192612.16</t>
+  </si>
+  <si>
+    <t>8.2721862E18</t>
   </si>
   <si>
     <t>GKD-b_48_n150_m45.txt</t>
   </si>
   <si>
-    <t>133032.23</t>
-  </si>
-  <si>
-    <t>-1.51447781E15</t>
+    <t>132279.84</t>
+  </si>
+  <si>
+    <t>8.2319809E18</t>
   </si>
   <si>
     <t>GKD-b_49_n150_m45.txt</t>
   </si>
   <si>
-    <t>194700.3</t>
-  </si>
-  <si>
-    <t>-1.51447795E15</t>
+    <t>195486.6</t>
+  </si>
+  <si>
+    <t>8.1860955E18</t>
   </si>
   <si>
     <t>GKD-b_4_n25_m2.txt</t>
@@ -890,118 +1091,133 @@
     <t>215.29823</t>
   </si>
   <si>
-    <t>-1.51447808E15</t>
+    <t>8.1445059E18</t>
   </si>
   <si>
     <t>GKD-b_50_n150_m45.txt</t>
   </si>
   <si>
-    <t>140946.33</t>
+    <t>142719.66</t>
+  </si>
+  <si>
+    <t>8.1386252E18</t>
   </si>
   <si>
     <t>GKD-b_5_n25_m2.txt</t>
   </si>
   <si>
-    <t>239.7942</t>
-  </si>
-  <si>
-    <t>-1.51447821E15</t>
+    <t>227.64333</t>
+  </si>
+  <si>
+    <t>8.0973798E18</t>
   </si>
   <si>
     <t>GKD-b_6_n25_m7.txt</t>
   </si>
   <si>
-    <t>4329.2114</t>
+    <t>4044.1936</t>
+  </si>
+  <si>
+    <t>8.092184E18</t>
   </si>
   <si>
     <t>GKD-b_7_n25_m7.txt</t>
   </si>
   <si>
-    <t>4170.243</t>
+    <t>4132.503</t>
+  </si>
+  <si>
+    <t>8.082267E18</t>
   </si>
   <si>
     <t>GKD-b_8_n25_m7.txt</t>
   </si>
   <si>
-    <t>3853.7422</t>
-  </si>
-  <si>
-    <t>-1.51447835E15</t>
+    <t>3768.208</t>
+  </si>
+  <si>
+    <t>8.0731361E18</t>
   </si>
   <si>
     <t>GKD-b_9_n25_m7.txt</t>
   </si>
   <si>
-    <t>1684.4073</t>
+    <t>1738.607</t>
+  </si>
+  <si>
+    <t>8.0644593E18</t>
   </si>
   <si>
     <t>GKD-c_10_n500_m50.txt</t>
   </si>
   <si>
-    <t>19130.934</t>
+    <t>18816.041</t>
+  </si>
+  <si>
+    <t>8.0553559E18</t>
   </si>
   <si>
     <t>GKD-c_11_n500_m50.txt</t>
   </si>
   <si>
-    <t>18785.598</t>
-  </si>
-  <si>
-    <t>-1.51447862E15</t>
+    <t>19004.834</t>
+  </si>
+  <si>
+    <t>7.9021098E18</t>
   </si>
   <si>
     <t>GKD-c_12_n500_m50.txt</t>
   </si>
   <si>
-    <t>18697.637</t>
-  </si>
-  <si>
-    <t>-1.51447875E15</t>
+    <t>18670.299</t>
+  </si>
+  <si>
+    <t>7.715046E18</t>
   </si>
   <si>
     <t>GKD-c_13_n500_m50.txt</t>
   </si>
   <si>
-    <t>18651.504</t>
-  </si>
-  <si>
-    <t>-1.51447902E15</t>
+    <t>18787.191</t>
+  </si>
+  <si>
+    <t>7.5176716E18</t>
   </si>
   <si>
     <t>GKD-c_14_n500_m50.txt</t>
   </si>
   <si>
-    <t>18609.42</t>
-  </si>
-  <si>
-    <t>-1.51447915E15</t>
+    <t>18682.162</t>
+  </si>
+  <si>
+    <t>7.3428537E18</t>
   </si>
   <si>
     <t>GKD-c_15_n500_m50.txt</t>
   </si>
   <si>
-    <t>18750.352</t>
-  </si>
-  <si>
-    <t>-1.51447942E15</t>
+    <t>18841.668</t>
+  </si>
+  <si>
+    <t>7.165238E18</t>
   </si>
   <si>
     <t>GKD-c_16_n500_m50.txt</t>
   </si>
   <si>
-    <t>19292.566</t>
-  </si>
-  <si>
-    <t>-1.51447956E15</t>
+    <t>19072.22</t>
+  </si>
+  <si>
+    <t>6.9787141E18</t>
   </si>
   <si>
     <t>GKD-c_17_n500_m50.txt</t>
   </si>
   <si>
-    <t>18570.332</t>
-  </si>
-  <si>
-    <t>-1.51447969E15</t>
+    <t>18789.77</t>
+  </si>
+  <si>
+    <t>6.8021028E18</t>
   </si>
   <si>
     <t>GKD-c_18_n500_m50.txt</t>
@@ -1010,106 +1226,106 @@
     <t>18846.688</t>
   </si>
   <si>
-    <t>-1.51447996E15</t>
+    <t>6.625402E18</t>
   </si>
   <si>
     <t>GKD-c_19_n500_m50.txt</t>
   </si>
   <si>
-    <t>19112.805</t>
-  </si>
-  <si>
-    <t>-1.51448009E15</t>
+    <t>18989.33</t>
+  </si>
+  <si>
+    <t>6.4438699E18</t>
   </si>
   <si>
     <t>GKD-c_1_n500_m50.txt</t>
   </si>
   <si>
-    <t>19100.902</t>
-  </si>
-  <si>
-    <t>-1.51448036E15</t>
+    <t>18956.22</t>
+  </si>
+  <si>
+    <t>6.2728051E18</t>
   </si>
   <si>
     <t>GKD-c_20_n500_m50.txt</t>
   </si>
   <si>
-    <t>19132.36</t>
-  </si>
-  <si>
-    <t>-1.5144805E15</t>
+    <t>19106.455</t>
+  </si>
+  <si>
+    <t>6.1065842E18</t>
   </si>
   <si>
     <t>GKD-c_2_n500_m50.txt</t>
   </si>
   <si>
-    <t>19088.283</t>
-  </si>
-  <si>
-    <t>-1.51448063E15</t>
+    <t>19257.027</t>
+  </si>
+  <si>
+    <t>5.9316426E18</t>
   </si>
   <si>
     <t>GKD-c_3_n500_m50.txt</t>
   </si>
   <si>
-    <t>18899.727</t>
-  </si>
-  <si>
-    <t>-1.5144809E15</t>
+    <t>18754.879</t>
+  </si>
+  <si>
+    <t>5.7849342E18</t>
   </si>
   <si>
     <t>GKD-c_4_n500_m50.txt</t>
   </si>
   <si>
-    <t>18795.64</t>
-  </si>
-  <si>
-    <t>-1.51448103E15</t>
+    <t>18678.963</t>
+  </si>
+  <si>
+    <t>5.6433446E18</t>
   </si>
   <si>
     <t>GKD-c_5_n500_m50.txt</t>
   </si>
   <si>
-    <t>18864.95</t>
-  </si>
-  <si>
-    <t>-1.5144813E15</t>
+    <t>18936.367</t>
+  </si>
+  <si>
+    <t>5.5022206E18</t>
   </si>
   <si>
     <t>GKD-c_6_n500_m50.txt</t>
   </si>
   <si>
-    <t>18983.574</t>
-  </si>
-  <si>
-    <t>-1.51448144E15</t>
+    <t>18937.74</t>
+  </si>
+  <si>
+    <t>5.3501549E18</t>
   </si>
   <si>
     <t>GKD-c_7_n500_m50.txt</t>
   </si>
   <si>
-    <t>18880.225</t>
-  </si>
-  <si>
-    <t>-1.5144817E15</t>
+    <t>18944.352</t>
+  </si>
+  <si>
+    <t>5.205281E18</t>
   </si>
   <si>
     <t>GKD-c_8_n500_m50.txt</t>
   </si>
   <si>
-    <t>18779.39</t>
-  </si>
-  <si>
-    <t>-1.51448184E15</t>
+    <t>18833.51</t>
+  </si>
+  <si>
+    <t>5.0443548E18</t>
   </si>
   <si>
     <t>GKD-c_9_n500_m50.txt</t>
   </si>
   <si>
-    <t>18655.98</t>
-  </si>
-  <si>
-    <t>-1.51448197E15</t>
+    <t>18748.047</t>
+  </si>
+  <si>
+    <t>4.8079192E18</t>
   </si>
   <si>
     <t>Promedio</t>
@@ -1204,1580 +1420,1580 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C34" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="B42" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="C42" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B43" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C44" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C46" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="C47" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="C48" t="s">
-        <v>117</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="C49" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>148</v>
       </c>
       <c r="C50" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>153</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C52" t="s">
-        <v>124</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B53" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="C53" t="s">
-        <v>131</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>160</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="B55" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="C55" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>139</v>
+        <v>168</v>
       </c>
       <c r="B57" t="s">
-        <v>140</v>
+        <v>169</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="B58" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>138</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>143</v>
+        <v>174</v>
       </c>
       <c r="B59" t="s">
-        <v>144</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
+        <v>176</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="B60" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>145</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="C61" t="s">
-        <v>150</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>151</v>
+        <v>183</v>
       </c>
       <c r="B62" t="s">
-        <v>152</v>
+        <v>184</v>
       </c>
       <c r="C62" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>153</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
-        <v>154</v>
+        <v>187</v>
       </c>
       <c r="C63" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
+        <v>190</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>192</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="B66" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>162</v>
+        <v>200</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>202</v>
       </c>
       <c r="C68" t="s">
-        <v>162</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>167</v>
+        <v>204</v>
       </c>
       <c r="B69" t="s">
-        <v>168</v>
+        <v>205</v>
       </c>
       <c r="C69" t="s">
-        <v>169</v>
+        <v>206</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>207</v>
       </c>
       <c r="B70" t="s">
-        <v>171</v>
+        <v>208</v>
       </c>
       <c r="C70" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="C71" t="s">
-        <v>169</v>
+        <v>212</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>174</v>
+        <v>213</v>
       </c>
       <c r="B72" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>177</v>
+        <v>216</v>
       </c>
       <c r="B73" t="s">
-        <v>178</v>
+        <v>217</v>
       </c>
       <c r="C73" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>179</v>
+        <v>219</v>
       </c>
       <c r="B74" t="s">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C74" t="s">
-        <v>181</v>
+        <v>221</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
       <c r="C75" t="s">
-        <v>181</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>184</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>185</v>
+        <v>226</v>
       </c>
       <c r="C76" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
-        <v>187</v>
+        <v>229</v>
       </c>
       <c r="C77" t="s">
-        <v>188</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>189</v>
+        <v>231</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="C78" t="s">
-        <v>188</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>191</v>
+        <v>234</v>
       </c>
       <c r="B79" t="s">
-        <v>192</v>
+        <v>235</v>
       </c>
       <c r="C79" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>193</v>
+        <v>237</v>
       </c>
       <c r="B80" t="s">
-        <v>194</v>
+        <v>238</v>
       </c>
       <c r="C80" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="C81" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="C82" t="s">
-        <v>197</v>
+        <v>245</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>200</v>
+        <v>246</v>
       </c>
       <c r="B83" t="s">
-        <v>201</v>
+        <v>247</v>
       </c>
       <c r="C83" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>202</v>
+        <v>249</v>
       </c>
       <c r="B84" t="s">
-        <v>203</v>
+        <v>250</v>
       </c>
       <c r="C84" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="B85" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
       <c r="C85" t="s">
-        <v>207</v>
+        <v>254</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>208</v>
+        <v>255</v>
       </c>
       <c r="B86" t="s">
-        <v>209</v>
+        <v>256</v>
       </c>
       <c r="C86" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>210</v>
+        <v>258</v>
       </c>
       <c r="B87" t="s">
-        <v>211</v>
+        <v>259</v>
       </c>
       <c r="C87" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>212</v>
+        <v>261</v>
       </c>
       <c r="B88" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
       <c r="C88" t="s">
-        <v>214</v>
+        <v>263</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>215</v>
+        <v>264</v>
       </c>
       <c r="B89" t="s">
-        <v>216</v>
+        <v>265</v>
       </c>
       <c r="C89" t="s">
-        <v>214</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="B90" t="s">
-        <v>218</v>
+        <v>268</v>
       </c>
       <c r="C90" t="s">
-        <v>214</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>270</v>
       </c>
       <c r="B91" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
       <c r="C91" t="s">
-        <v>214</v>
+        <v>272</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>273</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
+        <v>274</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>275</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>224</v>
+        <v>276</v>
       </c>
       <c r="B93" t="s">
-        <v>225</v>
+        <v>277</v>
       </c>
       <c r="C93" t="s">
-        <v>223</v>
+        <v>278</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>279</v>
       </c>
       <c r="B94" t="s">
-        <v>227</v>
+        <v>280</v>
       </c>
       <c r="C94" t="s">
-        <v>228</v>
+        <v>281</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>229</v>
+        <v>282</v>
       </c>
       <c r="B95" t="s">
-        <v>230</v>
+        <v>283</v>
       </c>
       <c r="C95" t="s">
-        <v>228</v>
+        <v>284</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>231</v>
+        <v>285</v>
       </c>
       <c r="B96" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="C96" t="s">
-        <v>228</v>
+        <v>287</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>233</v>
+        <v>288</v>
       </c>
       <c r="B97" t="s">
-        <v>234</v>
+        <v>289</v>
       </c>
       <c r="C97" t="s">
-        <v>235</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>236</v>
+        <v>291</v>
       </c>
       <c r="B98" t="s">
-        <v>237</v>
+        <v>292</v>
       </c>
       <c r="C98" t="s">
-        <v>235</v>
+        <v>293</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="B99" t="s">
-        <v>239</v>
+        <v>295</v>
       </c>
       <c r="C99" t="s">
-        <v>240</v>
+        <v>296</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>241</v>
+        <v>297</v>
       </c>
       <c r="B100" t="s">
-        <v>242</v>
+        <v>298</v>
       </c>
       <c r="C100" t="s">
-        <v>240</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>243</v>
+        <v>300</v>
       </c>
       <c r="B101" t="s">
-        <v>244</v>
+        <v>301</v>
       </c>
       <c r="C101" t="s">
-        <v>240</v>
+        <v>302</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>245</v>
+        <v>303</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>304</v>
       </c>
       <c r="C102" t="s">
-        <v>247</v>
+        <v>305</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>248</v>
+        <v>306</v>
       </c>
       <c r="B103" t="s">
-        <v>249</v>
+        <v>307</v>
       </c>
       <c r="C103" t="s">
-        <v>247</v>
+        <v>308</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>250</v>
+        <v>309</v>
       </c>
       <c r="B104" t="s">
-        <v>251</v>
+        <v>310</v>
       </c>
       <c r="C104" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>252</v>
+        <v>312</v>
       </c>
       <c r="B105" t="s">
-        <v>253</v>
+        <v>313</v>
       </c>
       <c r="C105" t="s">
-        <v>247</v>
+        <v>314</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>254</v>
+        <v>315</v>
       </c>
       <c r="B106" t="s">
-        <v>255</v>
+        <v>316</v>
       </c>
       <c r="C106" t="s">
-        <v>256</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>257</v>
+        <v>318</v>
       </c>
       <c r="B107" t="s">
-        <v>258</v>
+        <v>319</v>
       </c>
       <c r="C107" t="s">
-        <v>259</v>
+        <v>320</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>260</v>
+        <v>321</v>
       </c>
       <c r="B108" t="s">
-        <v>261</v>
+        <v>322</v>
       </c>
       <c r="C108" t="s">
-        <v>259</v>
+        <v>323</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>262</v>
+        <v>324</v>
       </c>
       <c r="B109" t="s">
-        <v>263</v>
+        <v>325</v>
       </c>
       <c r="C109" t="s">
-        <v>264</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>265</v>
+        <v>327</v>
       </c>
       <c r="B110" t="s">
-        <v>266</v>
+        <v>328</v>
       </c>
       <c r="C110" t="s">
-        <v>264</v>
+        <v>329</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>267</v>
+        <v>330</v>
       </c>
       <c r="B111" t="s">
-        <v>268</v>
+        <v>331</v>
       </c>
       <c r="C111" t="s">
-        <v>269</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>270</v>
+        <v>333</v>
       </c>
       <c r="B112" t="s">
-        <v>271</v>
+        <v>334</v>
       </c>
       <c r="C112" t="s">
-        <v>269</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>272</v>
+        <v>336</v>
       </c>
       <c r="B113" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="C113" t="s">
-        <v>274</v>
+        <v>338</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>275</v>
+        <v>339</v>
       </c>
       <c r="B114" t="s">
-        <v>276</v>
+        <v>340</v>
       </c>
       <c r="C114" t="s">
-        <v>274</v>
+        <v>341</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>277</v>
+        <v>342</v>
       </c>
       <c r="B115" t="s">
-        <v>278</v>
+        <v>343</v>
       </c>
       <c r="C115" t="s">
-        <v>274</v>
+        <v>344</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>279</v>
+        <v>345</v>
       </c>
       <c r="B116" t="s">
-        <v>280</v>
+        <v>346</v>
       </c>
       <c r="C116" t="s">
-        <v>281</v>
+        <v>347</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>282</v>
+        <v>348</v>
       </c>
       <c r="B117" t="s">
-        <v>283</v>
+        <v>349</v>
       </c>
       <c r="C117" t="s">
-        <v>281</v>
+        <v>350</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>284</v>
+        <v>351</v>
       </c>
       <c r="B118" t="s">
-        <v>285</v>
+        <v>352</v>
       </c>
       <c r="C118" t="s">
-        <v>286</v>
+        <v>353</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>287</v>
+        <v>354</v>
       </c>
       <c r="B119" t="s">
-        <v>288</v>
+        <v>355</v>
       </c>
       <c r="C119" t="s">
-        <v>289</v>
+        <v>356</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>290</v>
+        <v>357</v>
       </c>
       <c r="B120" t="s">
-        <v>291</v>
+        <v>358</v>
       </c>
       <c r="C120" t="s">
-        <v>292</v>
+        <v>359</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>293</v>
+        <v>360</v>
       </c>
       <c r="B121" t="s">
-        <v>294</v>
+        <v>361</v>
       </c>
       <c r="C121" t="s">
-        <v>292</v>
+        <v>362</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>295</v>
+        <v>363</v>
       </c>
       <c r="B122" t="s">
-        <v>296</v>
+        <v>364</v>
       </c>
       <c r="C122" t="s">
-        <v>297</v>
+        <v>365</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>298</v>
+        <v>366</v>
       </c>
       <c r="B123" t="s">
-        <v>299</v>
+        <v>367</v>
       </c>
       <c r="C123" t="s">
-        <v>297</v>
+        <v>368</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>300</v>
+        <v>369</v>
       </c>
       <c r="B124" t="s">
-        <v>301</v>
+        <v>370</v>
       </c>
       <c r="C124" t="s">
-        <v>297</v>
+        <v>371</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>302</v>
+        <v>372</v>
       </c>
       <c r="B125" t="s">
-        <v>303</v>
+        <v>373</v>
       </c>
       <c r="C125" t="s">
-        <v>304</v>
+        <v>374</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>305</v>
+        <v>375</v>
       </c>
       <c r="B126" t="s">
-        <v>306</v>
+        <v>376</v>
       </c>
       <c r="C126" t="s">
-        <v>304</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>307</v>
+        <v>378</v>
       </c>
       <c r="B127" t="s">
-        <v>308</v>
+        <v>379</v>
       </c>
       <c r="C127" t="s">
-        <v>304</v>
+        <v>380</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>309</v>
+        <v>381</v>
       </c>
       <c r="B128" t="s">
-        <v>310</v>
+        <v>382</v>
       </c>
       <c r="C128" t="s">
-        <v>311</v>
+        <v>383</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>312</v>
+        <v>384</v>
       </c>
       <c r="B129" t="s">
-        <v>313</v>
+        <v>385</v>
       </c>
       <c r="C129" t="s">
-        <v>314</v>
+        <v>386</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>315</v>
+        <v>387</v>
       </c>
       <c r="B130" t="s">
-        <v>316</v>
+        <v>388</v>
       </c>
       <c r="C130" t="s">
-        <v>317</v>
+        <v>389</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>318</v>
+        <v>390</v>
       </c>
       <c r="B131" t="s">
-        <v>319</v>
+        <v>391</v>
       </c>
       <c r="C131" t="s">
-        <v>320</v>
+        <v>392</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>321</v>
+        <v>393</v>
       </c>
       <c r="B132" t="s">
-        <v>322</v>
+        <v>394</v>
       </c>
       <c r="C132" t="s">
-        <v>323</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>324</v>
+        <v>396</v>
       </c>
       <c r="B133" t="s">
-        <v>325</v>
+        <v>397</v>
       </c>
       <c r="C133" t="s">
-        <v>326</v>
+        <v>398</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>327</v>
+        <v>399</v>
       </c>
       <c r="B134" t="s">
-        <v>328</v>
+        <v>400</v>
       </c>
       <c r="C134" t="s">
-        <v>329</v>
+        <v>401</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>330</v>
+        <v>402</v>
       </c>
       <c r="B135" t="s">
-        <v>331</v>
+        <v>403</v>
       </c>
       <c r="C135" t="s">
-        <v>332</v>
+        <v>404</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>333</v>
+        <v>405</v>
       </c>
       <c r="B136" t="s">
-        <v>334</v>
+        <v>406</v>
       </c>
       <c r="C136" t="s">
-        <v>335</v>
+        <v>407</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>336</v>
+        <v>408</v>
       </c>
       <c r="B137" t="s">
-        <v>337</v>
+        <v>409</v>
       </c>
       <c r="C137" t="s">
-        <v>338</v>
+        <v>410</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>339</v>
+        <v>411</v>
       </c>
       <c r="B138" t="s">
-        <v>340</v>
+        <v>412</v>
       </c>
       <c r="C138" t="s">
-        <v>341</v>
+        <v>413</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>342</v>
+        <v>414</v>
       </c>
       <c r="B139" t="s">
-        <v>343</v>
+        <v>415</v>
       </c>
       <c r="C139" t="s">
-        <v>344</v>
+        <v>416</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>345</v>
+        <v>417</v>
       </c>
       <c r="B140" t="s">
-        <v>346</v>
+        <v>418</v>
       </c>
       <c r="C140" t="s">
-        <v>347</v>
+        <v>419</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>348</v>
+        <v>420</v>
       </c>
       <c r="B141" t="s">
-        <v>349</v>
+        <v>421</v>
       </c>
       <c r="C141" t="s">
-        <v>350</v>
+        <v>422</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>351</v>
+        <v>423</v>
       </c>
       <c r="B142" t="s">
-        <v>352</v>
+        <v>424</v>
       </c>
       <c r="C142" t="s">
-        <v>353</v>
+        <v>425</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>354</v>
+        <v>426</v>
       </c>
       <c r="B143" t="s">
-        <v>355</v>
+        <v>427</v>
       </c>
       <c r="C143" t="s">
-        <v>356</v>
+        <v>428</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>357</v>
+        <v>429</v>
       </c>
       <c r="B144" t="s">
-        <v>358</v>
+        <v>430</v>
       </c>
       <c r="C144" t="s">
-        <v>359</v>
+        <v>431</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>360</v>
+        <v>432</v>
       </c>
       <c r="B145" t="s">
-        <v>361</v>
+        <v>433</v>
       </c>
       <c r="C145" t="s">
-        <v>362</v>
+        <v>434</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>435</v>
       </c>
       <c r="B146" t="s">
-        <v>364</v>
+        <v>436</v>
       </c>
       <c r="C146" t="s">
-        <v>365</v>
+        <v>437</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>366</v>
+        <v>438</v>
       </c>
       <c r="B147" t="n">
-        <v>19276.185546875</v>
+        <v>19263.765625</v>
       </c>
       <c r="C147" t="n">
-        <v>-1.514472845869056E15</v>
+        <v>1.49968878030972518E18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>